<commit_message>
tagged bitterroot pole #2 as rotated
</commit_message>
<xml_diff>
--- a/data/vgp_database/Bitterroot_Dome_intrusions.xlsx
+++ b/data/vgp_database/Bitterroot_Dome_intrusions.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjhWvTwszzS5RRhRbesg/UgMAZvnQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjFHPT+StMSNWcoty0c1XoNVDYrTA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="101">
   <si>
     <t>Name:</t>
   </si>
@@ -168,12 +168,6 @@
     <t>min age comes from Ar-Ar age from Hodges and Applegate (1993); max age comes from Ar-Ar age from Simonsen (1997). See Simonsen (1997) for additional Ar-Ar constraints from these dikes (which suggest they are mostly ~52 Ma).</t>
   </si>
   <si>
-    <t>Skalkaho intrusions</t>
-  </si>
-  <si>
-    <t>no pole position reported by original authors; some discussion of PSV and basic rock-mag; no field tests (R4=0); Skalkaho slab/block interpreted to have been strongly rotated about vertical axis so R5=-1</t>
-  </si>
-  <si>
     <t>Site level data</t>
   </si>
   <si>
@@ -298,6 +292,9 @@
   </si>
   <si>
     <t>S03</t>
+  </si>
+  <si>
+    <t>Skalkaho intrusions</t>
   </si>
   <si>
     <t>Results from these Skalkaho intrusions interpreted to have been rotated about a vertical axis on the basis of comparisons with 'reference ' directions from Diehl et al. (1983) (and are therefore not used for pole calculation above).</t>
@@ -461,14 +458,11 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -487,6 +481,9 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
@@ -1088,97 +1085,41 @@
       <c r="AO5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="21">
-        <v>8.0</v>
-      </c>
-      <c r="F6" s="21">
-        <v>46.4</v>
-      </c>
-      <c r="G6" s="21">
-        <v>69.1</v>
-      </c>
-      <c r="H6" s="21">
-        <v>18.1</v>
-      </c>
-      <c r="I6" s="21">
-        <v>13.4</v>
-      </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="16">
-        <v>46.4</v>
-      </c>
-      <c r="S6" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="T6" s="17">
-        <v>55.5</v>
-      </c>
-      <c r="U6" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="V6" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="W6" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="X6" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y6" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z6" s="17">
-        <v>1.0</v>
-      </c>
-      <c r="AA6" s="17">
-        <v>1.0</v>
-      </c>
-      <c r="AB6" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="AC6" s="17">
-        <v>1.0</v>
-      </c>
-      <c r="AD6" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="AE6" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="AF6" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="AG6" s="17">
-        <v>1.0</v>
-      </c>
-      <c r="AH6" s="17">
-        <v>1.0</v>
-      </c>
-      <c r="AI6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK6" s="19" t="s">
-        <v>51</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
       <c r="AL6" s="3"/>
       <c r="AM6" s="3"/>
       <c r="AN6" s="3"/>
@@ -1187,8 +1128,9 @@
       <c r="AQ6" s="3"/>
     </row>
     <row r="7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1219,6 +1161,8 @@
       <c r="AD7" s="3"/>
       <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
       <c r="AK7" s="3"/>
@@ -1230,207 +1174,262 @@
       <c r="AQ7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
-      <c r="AJ8" s="3"/>
-      <c r="AK8" s="3"/>
-      <c r="AL8" s="3"/>
-      <c r="AM8" s="3"/>
-      <c r="AN8" s="3"/>
-      <c r="AO8" s="3"/>
-      <c r="AP8" s="3"/>
-      <c r="AQ8" s="3"/>
+      <c r="F8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="U8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="V8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="X8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AL8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM8" s="10"/>
+      <c r="AN8" s="11"/>
+      <c r="AO8" s="11"/>
+      <c r="AP8" s="11"/>
+      <c r="AQ8" s="11"/>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="T9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="U9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="W9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="X9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC9" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF9" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG9" s="6" t="s">
+      <c r="A9" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="AH9" s="6" t="s">
+      <c r="B9" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="AI9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK9" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AL9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM9" s="10"/>
-      <c r="AN9" s="11"/>
-      <c r="AO9" s="11"/>
-      <c r="AP9" s="11"/>
-      <c r="AQ9" s="11"/>
+      <c r="C9" s="22">
+        <v>46.7</v>
+      </c>
+      <c r="D9" s="22">
+        <f t="shared" ref="D9:D13" si="1">360-114.6</f>
+        <v>245.4</v>
+      </c>
+      <c r="E9" s="23">
+        <v>4.0</v>
+      </c>
+      <c r="F9" s="23">
+        <v>336.9</v>
+      </c>
+      <c r="G9" s="23">
+        <v>65.7</v>
+      </c>
+      <c r="H9" s="22">
+        <v>94.5</v>
+      </c>
+      <c r="I9" s="23">
+        <v>9.5</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="23">
+        <v>74.2</v>
+      </c>
+      <c r="L9" s="23">
+        <v>169.6</v>
+      </c>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="16">
+        <v>46.4</v>
+      </c>
+      <c r="S9" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="T9" s="17">
+        <v>55.5</v>
+      </c>
+      <c r="U9" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="V9" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="W9" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="X9" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y9" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z9" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA9" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB9" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AE9" s="14"/>
+      <c r="AF9" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AG9" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="AH9" s="14"/>
+      <c r="AI9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="3"/>
     </row>
     <row r="10">
-      <c r="A10" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="23">
+      <c r="A10" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="22">
         <v>46.7</v>
       </c>
-      <c r="D10" s="23">
-        <f t="shared" ref="D10:D14" si="1">360-114.6</f>
+      <c r="D10" s="22">
+        <f t="shared" si="1"/>
         <v>245.4</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="23">
         <v>4.0</v>
       </c>
-      <c r="F10" s="24">
-        <v>336.9</v>
-      </c>
-      <c r="G10" s="24">
-        <v>65.7</v>
-      </c>
-      <c r="H10" s="23">
-        <v>94.5</v>
-      </c>
-      <c r="I10" s="24">
-        <v>9.5</v>
+      <c r="F10" s="23">
+        <v>342.8</v>
+      </c>
+      <c r="G10" s="23">
+        <v>66.9</v>
+      </c>
+      <c r="H10" s="22">
+        <v>60.4</v>
+      </c>
+      <c r="I10" s="23">
+        <v>11.9</v>
       </c>
       <c r="J10" s="14"/>
-      <c r="K10" s="24">
-        <v>74.2</v>
-      </c>
-      <c r="L10" s="24">
-        <v>169.6</v>
+      <c r="K10" s="23">
+        <v>78.3</v>
+      </c>
+      <c r="L10" s="23">
+        <v>175.6</v>
       </c>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
@@ -1459,10 +1458,10 @@
         <v>44</v>
       </c>
       <c r="Y10" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z10" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA10" s="17">
         <v>0.0</v>
@@ -1489,7 +1488,7 @@
         <v>47</v>
       </c>
       <c r="AK10" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL10" s="3" t="s">
         <v>49</v>
@@ -1498,40 +1497,40 @@
       <c r="AN10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="23">
+      <c r="A11" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="22">
         <v>46.7</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="22">
         <f t="shared" si="1"/>
         <v>245.4</v>
       </c>
-      <c r="E11" s="24">
-        <v>4.0</v>
-      </c>
-      <c r="F11" s="24">
-        <v>342.8</v>
-      </c>
-      <c r="G11" s="24">
-        <v>66.9</v>
-      </c>
-      <c r="H11" s="23">
-        <v>60.4</v>
-      </c>
-      <c r="I11" s="24">
-        <v>11.9</v>
+      <c r="E11" s="23">
+        <v>7.0</v>
+      </c>
+      <c r="F11" s="23">
+        <v>324.8</v>
+      </c>
+      <c r="G11" s="23">
+        <v>59.0</v>
+      </c>
+      <c r="H11" s="22">
+        <v>256.8</v>
+      </c>
+      <c r="I11" s="23">
+        <v>3.8</v>
       </c>
       <c r="J11" s="14"/>
-      <c r="K11" s="24">
-        <v>78.3</v>
-      </c>
-      <c r="L11" s="24">
-        <v>175.6</v>
+      <c r="K11" s="23">
+        <v>63.8</v>
+      </c>
+      <c r="L11" s="23">
+        <v>153.3</v>
       </c>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
@@ -1560,10 +1559,10 @@
         <v>44</v>
       </c>
       <c r="Y11" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z11" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA11" s="17">
         <v>0.0</v>
@@ -1590,7 +1589,7 @@
         <v>47</v>
       </c>
       <c r="AK11" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL11" s="3" t="s">
         <v>49</v>
@@ -1599,40 +1598,40 @@
       <c r="AN11" s="3"/>
     </row>
     <row r="12">
-      <c r="A12" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="23">
+      <c r="A12" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="22">
         <v>46.7</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="22">
         <f t="shared" si="1"/>
         <v>245.4</v>
       </c>
-      <c r="E12" s="24">
-        <v>7.0</v>
-      </c>
-      <c r="F12" s="24">
-        <v>324.8</v>
-      </c>
-      <c r="G12" s="24">
-        <v>59.0</v>
-      </c>
-      <c r="H12" s="23">
-        <v>256.8</v>
-      </c>
-      <c r="I12" s="24">
-        <v>3.8</v>
+      <c r="E12" s="23">
+        <v>5.0</v>
+      </c>
+      <c r="F12" s="23">
+        <v>331.4</v>
+      </c>
+      <c r="G12" s="23">
+        <v>59.2</v>
+      </c>
+      <c r="H12" s="22">
+        <v>48.6</v>
+      </c>
+      <c r="I12" s="23">
+        <v>11.1</v>
       </c>
       <c r="J12" s="14"/>
-      <c r="K12" s="24">
-        <v>63.8</v>
-      </c>
-      <c r="L12" s="24">
-        <v>153.3</v>
+      <c r="K12" s="23">
+        <v>69.4</v>
+      </c>
+      <c r="L12" s="23">
+        <v>150.2</v>
       </c>
       <c r="M12" s="14"/>
       <c r="N12" s="14"/>
@@ -1661,10 +1660,10 @@
         <v>44</v>
       </c>
       <c r="Y12" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z12" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA12" s="17">
         <v>0.0</v>
@@ -1691,7 +1690,7 @@
         <v>47</v>
       </c>
       <c r="AK12" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL12" s="3" t="s">
         <v>49</v>
@@ -1700,40 +1699,40 @@
       <c r="AN12" s="3"/>
     </row>
     <row r="13">
-      <c r="A13" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="23">
+      <c r="A13" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="22">
         <v>46.7</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <f t="shared" si="1"/>
         <v>245.4</v>
       </c>
-      <c r="E13" s="24">
-        <v>5.0</v>
-      </c>
-      <c r="F13" s="24">
-        <v>331.4</v>
-      </c>
-      <c r="G13" s="24">
-        <v>59.2</v>
-      </c>
-      <c r="H13" s="23">
-        <v>48.6</v>
-      </c>
-      <c r="I13" s="24">
-        <v>11.1</v>
+      <c r="E13" s="23">
+        <v>3.0</v>
+      </c>
+      <c r="F13" s="23">
+        <v>327.1</v>
+      </c>
+      <c r="G13" s="23">
+        <v>50.9</v>
+      </c>
+      <c r="H13" s="22">
+        <v>144.3</v>
+      </c>
+      <c r="I13" s="23">
+        <v>10.3</v>
       </c>
       <c r="J13" s="14"/>
-      <c r="K13" s="24">
-        <v>69.4</v>
-      </c>
-      <c r="L13" s="24">
-        <v>150.2</v>
+      <c r="K13" s="23">
+        <v>60.7</v>
+      </c>
+      <c r="L13" s="23">
+        <v>136.3</v>
       </c>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
@@ -1762,10 +1761,10 @@
         <v>44</v>
       </c>
       <c r="Y13" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z13" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA13" s="17">
         <v>0.0</v>
@@ -1792,7 +1791,7 @@
         <v>47</v>
       </c>
       <c r="AK13" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL13" s="3" t="s">
         <v>49</v>
@@ -1801,40 +1800,40 @@
       <c r="AN13" s="3"/>
     </row>
     <row r="14">
-      <c r="A14" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="23">
-        <v>46.7</v>
-      </c>
-      <c r="D14" s="23">
-        <f t="shared" si="1"/>
-        <v>245.4</v>
-      </c>
-      <c r="E14" s="24">
-        <v>3.0</v>
-      </c>
-      <c r="F14" s="24">
-        <v>327.1</v>
-      </c>
-      <c r="G14" s="24">
-        <v>50.9</v>
-      </c>
-      <c r="H14" s="23">
-        <v>144.3</v>
-      </c>
-      <c r="I14" s="24">
-        <v>10.3</v>
+      <c r="A14" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="22">
+        <v>46.1</v>
+      </c>
+      <c r="D14" s="22">
+        <f t="shared" ref="D14:D17" si="2">360-115.2</f>
+        <v>244.8</v>
+      </c>
+      <c r="E14" s="23">
+        <v>2.0</v>
+      </c>
+      <c r="F14" s="23">
+        <v>171.7</v>
+      </c>
+      <c r="G14" s="23">
+        <v>-64.6</v>
+      </c>
+      <c r="H14" s="22">
+        <v>50.5</v>
+      </c>
+      <c r="I14" s="23">
+        <v>35.9</v>
       </c>
       <c r="J14" s="14"/>
-      <c r="K14" s="24">
-        <v>60.7</v>
-      </c>
-      <c r="L14" s="24">
-        <v>136.3</v>
+      <c r="K14" s="23">
+        <v>-84.2</v>
+      </c>
+      <c r="L14" s="23">
+        <v>-17.6</v>
       </c>
       <c r="M14" s="14"/>
       <c r="N14" s="14"/>
@@ -1863,10 +1862,10 @@
         <v>44</v>
       </c>
       <c r="Y14" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z14" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA14" s="17">
         <v>0.0</v>
@@ -1879,8 +1878,8 @@
         <v>0.0</v>
       </c>
       <c r="AE14" s="14"/>
-      <c r="AF14" s="17">
-        <v>0.0</v>
+      <c r="AF14" s="18" t="s">
+        <v>74</v>
       </c>
       <c r="AG14" s="16">
         <v>1.0</v>
@@ -1893,7 +1892,7 @@
         <v>47</v>
       </c>
       <c r="AK14" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL14" s="3" t="s">
         <v>49</v>
@@ -1902,40 +1901,40 @@
       <c r="AN14" s="3"/>
     </row>
     <row r="15">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="23">
+      <c r="B15" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="22">
         <v>46.1</v>
       </c>
-      <c r="D15" s="23">
-        <f t="shared" ref="D15:D18" si="2">360-115.2</f>
+      <c r="D15" s="22">
+        <f t="shared" si="2"/>
         <v>244.8</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="13">
         <v>2.0</v>
       </c>
-      <c r="F15" s="24">
-        <v>171.7</v>
-      </c>
-      <c r="G15" s="24">
-        <v>-64.6</v>
-      </c>
-      <c r="H15" s="23">
-        <v>50.5</v>
-      </c>
-      <c r="I15" s="24">
-        <v>35.9</v>
+      <c r="F15" s="13">
+        <v>166.5</v>
+      </c>
+      <c r="G15" s="13">
+        <v>-72.5</v>
+      </c>
+      <c r="H15" s="13">
+        <v>172.9</v>
+      </c>
+      <c r="I15" s="13">
+        <v>19.1</v>
       </c>
       <c r="J15" s="14"/>
-      <c r="K15" s="24">
-        <v>-84.2</v>
-      </c>
-      <c r="L15" s="24">
-        <v>-17.6</v>
+      <c r="K15" s="16">
+        <v>-75.7</v>
+      </c>
+      <c r="L15" s="16">
+        <v>34.6</v>
       </c>
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
@@ -1964,10 +1963,10 @@
         <v>44</v>
       </c>
       <c r="Y15" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z15" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA15" s="17">
         <v>0.0</v>
@@ -1980,13 +1979,15 @@
         <v>0.0</v>
       </c>
       <c r="AE15" s="14"/>
-      <c r="AF15" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG15" s="16">
+      <c r="AF15" s="18">
         <v>1.0</v>
       </c>
-      <c r="AH15" s="14"/>
+      <c r="AG15" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="AH15" s="24">
+        <v>12.0</v>
+      </c>
       <c r="AI15" s="3" t="s">
         <v>46</v>
       </c>
@@ -1994,7 +1995,7 @@
         <v>47</v>
       </c>
       <c r="AK15" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL15" s="3" t="s">
         <v>49</v>
@@ -2003,16 +2004,16 @@
       <c r="AN15" s="3"/>
     </row>
     <row r="16">
-      <c r="A16" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="23">
+      <c r="A16" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="22">
         <v>46.1</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="22">
         <f t="shared" si="2"/>
         <v>244.8</v>
       </c>
@@ -2020,23 +2021,23 @@
         <v>2.0</v>
       </c>
       <c r="F16" s="13">
-        <v>166.5</v>
+        <v>174.5</v>
       </c>
       <c r="G16" s="13">
-        <v>-72.5</v>
+        <v>-56.7</v>
       </c>
       <c r="H16" s="13">
-        <v>172.9</v>
+        <v>231.4</v>
       </c>
       <c r="I16" s="13">
-        <v>19.1</v>
+        <v>16.5</v>
       </c>
       <c r="J16" s="14"/>
       <c r="K16" s="16">
-        <v>-75.7</v>
+        <v>-80.3</v>
       </c>
       <c r="L16" s="16">
-        <v>34.6</v>
+        <v>-88.2</v>
       </c>
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
@@ -2065,10 +2066,10 @@
         <v>44</v>
       </c>
       <c r="Y16" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z16" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA16" s="17">
         <v>0.0</v>
@@ -2084,10 +2085,10 @@
       <c r="AF16" s="18">
         <v>1.0</v>
       </c>
-      <c r="AG16" s="25">
+      <c r="AG16" s="24">
         <v>0.0</v>
       </c>
-      <c r="AH16" s="25">
+      <c r="AH16" s="24">
         <v>12.0</v>
       </c>
       <c r="AI16" s="3" t="s">
@@ -2097,7 +2098,7 @@
         <v>47</v>
       </c>
       <c r="AK16" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL16" s="3" t="s">
         <v>49</v>
@@ -2106,40 +2107,40 @@
       <c r="AN16" s="3"/>
     </row>
     <row r="17">
-      <c r="A17" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="23">
+      <c r="A17" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="22">
         <v>46.1</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="22">
         <f t="shared" si="2"/>
         <v>244.8</v>
       </c>
-      <c r="E17" s="13">
-        <v>2.0</v>
-      </c>
-      <c r="F17" s="13">
-        <v>174.5</v>
-      </c>
-      <c r="G17" s="13">
-        <v>-56.7</v>
-      </c>
-      <c r="H17" s="13">
-        <v>231.4</v>
-      </c>
-      <c r="I17" s="13">
-        <v>16.5</v>
+      <c r="E17" s="23">
+        <v>3.0</v>
+      </c>
+      <c r="F17" s="23">
+        <v>344.0</v>
+      </c>
+      <c r="G17" s="23">
+        <v>71.4</v>
+      </c>
+      <c r="H17" s="22">
+        <v>48.5</v>
+      </c>
+      <c r="I17" s="23">
+        <v>17.9</v>
       </c>
       <c r="J17" s="14"/>
-      <c r="K17" s="16">
-        <v>-80.3</v>
-      </c>
-      <c r="L17" s="16">
-        <v>-88.2</v>
+      <c r="K17" s="25">
+        <v>75.9</v>
+      </c>
+      <c r="L17" s="25">
+        <v>-154.3</v>
       </c>
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
@@ -2168,10 +2169,10 @@
         <v>44</v>
       </c>
       <c r="Y17" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z17" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA17" s="17">
         <v>0.0</v>
@@ -2184,15 +2185,13 @@
         <v>0.0</v>
       </c>
       <c r="AE17" s="14"/>
-      <c r="AF17" s="18">
+      <c r="AF17" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AG17" s="16">
         <v>1.0</v>
       </c>
-      <c r="AG17" s="25">
-        <v>0.0</v>
-      </c>
-      <c r="AH17" s="25">
-        <v>12.0</v>
-      </c>
+      <c r="AH17" s="14"/>
       <c r="AI17" s="3" t="s">
         <v>46</v>
       </c>
@@ -2200,7 +2199,7 @@
         <v>47</v>
       </c>
       <c r="AK17" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL17" s="3" t="s">
         <v>49</v>
@@ -2209,40 +2208,40 @@
       <c r="AN17" s="3"/>
     </row>
     <row r="18">
-      <c r="A18" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="23">
+      <c r="A18" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="22">
         <v>46.1</v>
       </c>
-      <c r="D18" s="23">
-        <f t="shared" si="2"/>
-        <v>244.8</v>
-      </c>
-      <c r="E18" s="24">
-        <v>3.0</v>
-      </c>
-      <c r="F18" s="24">
-        <v>344.0</v>
-      </c>
-      <c r="G18" s="24">
-        <v>71.4</v>
-      </c>
-      <c r="H18" s="23">
-        <v>48.5</v>
-      </c>
-      <c r="I18" s="24">
-        <v>17.9</v>
+      <c r="D18" s="22">
+        <f t="shared" ref="D18:D27" si="3">360-115.1</f>
+        <v>244.9</v>
+      </c>
+      <c r="E18" s="23">
+        <v>2.0</v>
+      </c>
+      <c r="F18" s="23">
+        <v>328.1</v>
+      </c>
+      <c r="G18" s="23">
+        <v>78.1</v>
+      </c>
+      <c r="H18" s="22">
+        <v>30.0</v>
+      </c>
+      <c r="I18" s="23">
+        <v>47.3</v>
       </c>
       <c r="J18" s="14"/>
-      <c r="K18" s="26">
-        <v>75.9</v>
-      </c>
-      <c r="L18" s="26">
-        <v>-154.3</v>
+      <c r="K18" s="25">
+        <v>63.2</v>
+      </c>
+      <c r="L18" s="25">
+        <v>-142.2</v>
       </c>
       <c r="M18" s="14"/>
       <c r="N18" s="14"/>
@@ -2271,10 +2270,10 @@
         <v>44</v>
       </c>
       <c r="Y18" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z18" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA18" s="17">
         <v>0.0</v>
@@ -2287,8 +2286,8 @@
         <v>0.0</v>
       </c>
       <c r="AE18" s="14"/>
-      <c r="AF18" s="17">
-        <v>0.0</v>
+      <c r="AF18" s="18" t="s">
+        <v>79</v>
       </c>
       <c r="AG18" s="16">
         <v>1.0</v>
@@ -2301,7 +2300,7 @@
         <v>47</v>
       </c>
       <c r="AK18" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL18" s="3" t="s">
         <v>49</v>
@@ -2310,40 +2309,38 @@
       <c r="AN18" s="3"/>
     </row>
     <row r="19">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="23">
+      <c r="B19" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="22">
         <v>46.1</v>
       </c>
-      <c r="D19" s="23">
-        <f t="shared" ref="D19:D28" si="3">360-115.1</f>
+      <c r="D19" s="22">
+        <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E19" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="F19" s="24">
-        <v>328.1</v>
-      </c>
-      <c r="G19" s="24">
-        <v>78.1</v>
-      </c>
-      <c r="H19" s="23">
-        <v>30.0</v>
-      </c>
-      <c r="I19" s="24">
-        <v>47.3</v>
+      <c r="E19" s="23">
+        <v>4.0</v>
+      </c>
+      <c r="F19" s="23">
+        <v>268.3</v>
+      </c>
+      <c r="G19" s="23">
+        <v>81.8</v>
+      </c>
+      <c r="H19" s="26"/>
+      <c r="I19" s="23">
+        <v>13.3</v>
       </c>
       <c r="J19" s="14"/>
-      <c r="K19" s="26">
-        <v>63.2</v>
-      </c>
-      <c r="L19" s="26">
-        <v>-142.2</v>
+      <c r="K19" s="25">
+        <v>43.3</v>
+      </c>
+      <c r="L19" s="25">
+        <v>-137.5</v>
       </c>
       <c r="M19" s="14"/>
       <c r="N19" s="14"/>
@@ -2372,10 +2369,10 @@
         <v>44</v>
       </c>
       <c r="Y19" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z19" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA19" s="17">
         <v>0.0</v>
@@ -2388,13 +2385,15 @@
         <v>0.0</v>
       </c>
       <c r="AE19" s="14"/>
-      <c r="AF19" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG19" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="AH19" s="14"/>
+      <c r="AF19" s="18">
+        <v>2.0</v>
+      </c>
+      <c r="AG19" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="AH19" s="24">
+        <v>12.0</v>
+      </c>
       <c r="AI19" s="3" t="s">
         <v>46</v>
       </c>
@@ -2402,7 +2401,7 @@
         <v>47</v>
       </c>
       <c r="AK19" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL19" s="3" t="s">
         <v>49</v>
@@ -2411,38 +2410,40 @@
       <c r="AN19" s="3"/>
     </row>
     <row r="20">
-      <c r="A20" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="23">
+      <c r="A20" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="22">
         <v>46.1</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="22">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="13">
         <v>4.0</v>
       </c>
-      <c r="F20" s="24">
-        <v>268.3</v>
-      </c>
-      <c r="G20" s="24">
-        <v>81.8</v>
-      </c>
-      <c r="H20" s="27"/>
-      <c r="I20" s="24">
-        <v>13.3</v>
+      <c r="F20" s="13">
+        <v>348.4</v>
+      </c>
+      <c r="G20" s="13">
+        <v>69.2</v>
+      </c>
+      <c r="H20" s="13">
+        <v>126.0</v>
+      </c>
+      <c r="I20" s="13">
+        <v>11.0</v>
       </c>
       <c r="J20" s="14"/>
-      <c r="K20" s="26">
-        <v>43.3</v>
-      </c>
-      <c r="L20" s="26">
-        <v>-137.5</v>
+      <c r="K20" s="16">
+        <v>80.0</v>
+      </c>
+      <c r="L20" s="16">
+        <v>-159.3</v>
       </c>
       <c r="M20" s="14"/>
       <c r="N20" s="14"/>
@@ -2471,10 +2472,10 @@
         <v>44</v>
       </c>
       <c r="Y20" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z20" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA20" s="17">
         <v>0.0</v>
@@ -2490,10 +2491,10 @@
       <c r="AF20" s="18">
         <v>2.0</v>
       </c>
-      <c r="AG20" s="25">
+      <c r="AG20" s="24">
         <v>0.0</v>
       </c>
-      <c r="AH20" s="25">
+      <c r="AH20" s="24">
         <v>12.0</v>
       </c>
       <c r="AI20" s="3" t="s">
@@ -2503,7 +2504,7 @@
         <v>47</v>
       </c>
       <c r="AK20" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL20" s="3" t="s">
         <v>49</v>
@@ -2512,40 +2513,40 @@
       <c r="AN20" s="3"/>
     </row>
     <row r="21">
-      <c r="A21" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="23">
+      <c r="A21" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="22">
         <v>46.1</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="22">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E21" s="13">
-        <v>4.0</v>
-      </c>
-      <c r="F21" s="13">
-        <v>348.4</v>
-      </c>
-      <c r="G21" s="13">
-        <v>69.2</v>
-      </c>
-      <c r="H21" s="13">
-        <v>126.0</v>
-      </c>
-      <c r="I21" s="13">
-        <v>11.0</v>
+      <c r="E21" s="23">
+        <v>2.0</v>
+      </c>
+      <c r="F21" s="23">
+        <v>163.0</v>
+      </c>
+      <c r="G21" s="23">
+        <v>-57.7</v>
+      </c>
+      <c r="H21" s="22">
+        <v>1362.9</v>
+      </c>
+      <c r="I21" s="23">
+        <v>6.8</v>
       </c>
       <c r="J21" s="14"/>
-      <c r="K21" s="16">
-        <v>80.0</v>
-      </c>
-      <c r="L21" s="16">
-        <v>-159.3</v>
+      <c r="K21" s="25">
+        <v>-75.5</v>
+      </c>
+      <c r="L21" s="25">
+        <v>-50.8</v>
       </c>
       <c r="M21" s="14"/>
       <c r="N21" s="14"/>
@@ -2574,10 +2575,10 @@
         <v>44</v>
       </c>
       <c r="Y21" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z21" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA21" s="17">
         <v>0.0</v>
@@ -2590,15 +2591,13 @@
         <v>0.0</v>
       </c>
       <c r="AE21" s="14"/>
-      <c r="AF21" s="18">
-        <v>2.0</v>
-      </c>
-      <c r="AG21" s="25">
-        <v>0.0</v>
-      </c>
-      <c r="AH21" s="25">
-        <v>12.0</v>
-      </c>
+      <c r="AF21" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG21" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="AH21" s="14"/>
       <c r="AI21" s="3" t="s">
         <v>46</v>
       </c>
@@ -2606,7 +2605,7 @@
         <v>47</v>
       </c>
       <c r="AK21" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL21" s="3" t="s">
         <v>49</v>
@@ -2615,40 +2614,40 @@
       <c r="AN21" s="3"/>
     </row>
     <row r="22">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="23">
+      <c r="B22" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="22">
         <v>46.1</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="22">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E22" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="F22" s="24">
-        <v>163.0</v>
-      </c>
-      <c r="G22" s="24">
+      <c r="E22" s="23">
+        <v>5.0</v>
+      </c>
+      <c r="F22" s="23">
+        <v>160.1</v>
+      </c>
+      <c r="G22" s="23">
         <v>-57.7</v>
       </c>
-      <c r="H22" s="23">
-        <v>1362.9</v>
-      </c>
-      <c r="I22" s="24">
-        <v>6.8</v>
+      <c r="H22" s="22">
+        <v>333.0</v>
+      </c>
+      <c r="I22" s="23">
+        <v>4.2</v>
       </c>
       <c r="J22" s="14"/>
-      <c r="K22" s="26">
-        <v>-75.5</v>
-      </c>
-      <c r="L22" s="26">
-        <v>-50.8</v>
+      <c r="K22" s="25">
+        <v>-73.4</v>
+      </c>
+      <c r="L22" s="25">
+        <v>-45.7</v>
       </c>
       <c r="M22" s="14"/>
       <c r="N22" s="14"/>
@@ -2677,10 +2676,10 @@
         <v>44</v>
       </c>
       <c r="Y22" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z22" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA22" s="17">
         <v>0.0</v>
@@ -2693,13 +2692,15 @@
         <v>0.0</v>
       </c>
       <c r="AE22" s="14"/>
-      <c r="AF22" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG22" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="AH22" s="14"/>
+      <c r="AF22" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="AG22" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="AH22" s="24">
+        <v>12.0</v>
+      </c>
       <c r="AI22" s="3" t="s">
         <v>46</v>
       </c>
@@ -2707,7 +2708,7 @@
         <v>47</v>
       </c>
       <c r="AK22" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL22" s="3" t="s">
         <v>49</v>
@@ -2716,40 +2717,40 @@
       <c r="AN22" s="3"/>
     </row>
     <row r="23">
-      <c r="A23" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="23">
+      <c r="A23" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="22">
         <v>46.1</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="22">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E23" s="24">
-        <v>5.0</v>
-      </c>
-      <c r="F23" s="24">
-        <v>160.1</v>
-      </c>
-      <c r="G23" s="24">
-        <v>-57.7</v>
-      </c>
-      <c r="H23" s="23">
-        <v>333.0</v>
-      </c>
-      <c r="I23" s="24">
-        <v>4.2</v>
+      <c r="E23" s="23">
+        <v>3.0</v>
+      </c>
+      <c r="F23" s="23">
+        <v>165.9</v>
+      </c>
+      <c r="G23" s="23">
+        <v>-57.6</v>
+      </c>
+      <c r="H23" s="22">
+        <v>3905.3</v>
+      </c>
+      <c r="I23" s="23">
+        <v>2.0</v>
       </c>
       <c r="J23" s="14"/>
-      <c r="K23" s="26">
-        <v>-73.4</v>
-      </c>
-      <c r="L23" s="26">
-        <v>-45.7</v>
+      <c r="K23" s="25">
+        <v>-77.0</v>
+      </c>
+      <c r="L23" s="25">
+        <v>-56.9</v>
       </c>
       <c r="M23" s="14"/>
       <c r="N23" s="14"/>
@@ -2778,10 +2779,10 @@
         <v>44</v>
       </c>
       <c r="Y23" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z23" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA23" s="17">
         <v>0.0</v>
@@ -2797,10 +2798,10 @@
       <c r="AF23" s="18">
         <v>3.0</v>
       </c>
-      <c r="AG23" s="25">
+      <c r="AG23" s="24">
         <v>0.0</v>
       </c>
-      <c r="AH23" s="25">
+      <c r="AH23" s="24">
         <v>12.0</v>
       </c>
       <c r="AI23" s="3" t="s">
@@ -2810,7 +2811,7 @@
         <v>47</v>
       </c>
       <c r="AK23" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL23" s="3" t="s">
         <v>49</v>
@@ -2819,40 +2820,40 @@
       <c r="AN23" s="3"/>
     </row>
     <row r="24">
-      <c r="A24" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="23">
+      <c r="A24" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="22">
         <v>46.1</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="22">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E24" s="24">
-        <v>3.0</v>
-      </c>
-      <c r="F24" s="24">
-        <v>165.9</v>
-      </c>
-      <c r="G24" s="24">
-        <v>-57.6</v>
-      </c>
-      <c r="H24" s="23">
-        <v>3905.3</v>
-      </c>
-      <c r="I24" s="24">
+      <c r="E24" s="23">
         <v>2.0</v>
       </c>
+      <c r="F24" s="23">
+        <v>120.3</v>
+      </c>
+      <c r="G24" s="23">
+        <v>-66.9</v>
+      </c>
+      <c r="H24" s="22">
+        <v>40.4</v>
+      </c>
+      <c r="I24" s="23">
+        <v>40.4</v>
+      </c>
       <c r="J24" s="14"/>
-      <c r="K24" s="26">
-        <v>-77.0</v>
-      </c>
-      <c r="L24" s="26">
-        <v>-56.9</v>
+      <c r="K24" s="25">
+        <v>-50.9</v>
+      </c>
+      <c r="L24" s="25">
+        <v>2.5</v>
       </c>
       <c r="M24" s="14"/>
       <c r="N24" s="14"/>
@@ -2881,10 +2882,10 @@
         <v>44</v>
       </c>
       <c r="Y24" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z24" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA24" s="17">
         <v>0.0</v>
@@ -2897,15 +2898,13 @@
         <v>0.0</v>
       </c>
       <c r="AE24" s="14"/>
-      <c r="AF24" s="18">
-        <v>3.0</v>
-      </c>
-      <c r="AG24" s="25">
-        <v>0.0</v>
-      </c>
-      <c r="AH24" s="25">
-        <v>12.0</v>
-      </c>
+      <c r="AF24" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG24" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="AH24" s="14"/>
       <c r="AI24" s="3" t="s">
         <v>46</v>
       </c>
@@ -2913,7 +2912,7 @@
         <v>47</v>
       </c>
       <c r="AK24" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL24" s="3" t="s">
         <v>49</v>
@@ -2922,40 +2921,38 @@
       <c r="AN24" s="3"/>
     </row>
     <row r="25">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="23">
+      <c r="B25" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="22">
         <v>46.1</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="22">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E25" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="F25" s="24">
-        <v>120.3</v>
-      </c>
-      <c r="G25" s="24">
-        <v>-66.9</v>
-      </c>
-      <c r="H25" s="23">
-        <v>40.4</v>
-      </c>
-      <c r="I25" s="24">
-        <v>40.4</v>
+      <c r="E25" s="23">
+        <v>5.0</v>
+      </c>
+      <c r="F25" s="23">
+        <v>99.3</v>
+      </c>
+      <c r="G25" s="23">
+        <v>-64.3</v>
+      </c>
+      <c r="H25" s="26"/>
+      <c r="I25" s="23">
+        <v>6.9</v>
       </c>
       <c r="J25" s="14"/>
-      <c r="K25" s="26">
-        <v>-50.9</v>
-      </c>
-      <c r="L25" s="26">
-        <v>2.5</v>
+      <c r="K25" s="25">
+        <v>-36.6</v>
+      </c>
+      <c r="L25" s="27">
+        <v>6.5</v>
       </c>
       <c r="M25" s="14"/>
       <c r="N25" s="14"/>
@@ -2984,10 +2981,10 @@
         <v>44</v>
       </c>
       <c r="Y25" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z25" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA25" s="17">
         <v>0.0</v>
@@ -3000,13 +2997,15 @@
         <v>0.0</v>
       </c>
       <c r="AE25" s="14"/>
-      <c r="AF25" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="AG25" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="AH25" s="14"/>
+      <c r="AF25" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="AG25" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="AH25" s="24">
+        <v>12.0</v>
+      </c>
       <c r="AI25" s="3" t="s">
         <v>46</v>
       </c>
@@ -3014,7 +3013,7 @@
         <v>47</v>
       </c>
       <c r="AK25" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL25" s="3" t="s">
         <v>49</v>
@@ -3023,38 +3022,40 @@
       <c r="AN25" s="3"/>
     </row>
     <row r="26">
-      <c r="A26" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="23">
+      <c r="A26" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="22">
         <v>46.1</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="22">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E26" s="24">
-        <v>5.0</v>
-      </c>
-      <c r="F26" s="24">
-        <v>99.3</v>
-      </c>
-      <c r="G26" s="24">
-        <v>-64.3</v>
-      </c>
-      <c r="H26" s="27"/>
-      <c r="I26" s="24">
-        <v>6.9</v>
+      <c r="E26" s="23">
+        <v>2.0</v>
+      </c>
+      <c r="F26" s="23">
+        <v>143.2</v>
+      </c>
+      <c r="G26" s="23">
+        <v>-66.4</v>
+      </c>
+      <c r="H26" s="22">
+        <v>4447.8</v>
+      </c>
+      <c r="I26" s="23">
+        <v>3.8</v>
       </c>
       <c r="J26" s="14"/>
-      <c r="K26" s="26">
-        <v>-36.6</v>
-      </c>
-      <c r="L26" s="28">
-        <v>6.5</v>
+      <c r="K26" s="25">
+        <v>-65.2</v>
+      </c>
+      <c r="L26" s="25">
+        <v>-5.2</v>
       </c>
       <c r="M26" s="14"/>
       <c r="N26" s="14"/>
@@ -3083,10 +3084,10 @@
         <v>44</v>
       </c>
       <c r="Y26" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z26" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA26" s="17">
         <v>0.0</v>
@@ -3102,10 +3103,10 @@
       <c r="AF26" s="18">
         <v>4.0</v>
       </c>
-      <c r="AG26" s="25">
+      <c r="AG26" s="24">
         <v>0.0</v>
       </c>
-      <c r="AH26" s="25">
+      <c r="AH26" s="24">
         <v>12.0</v>
       </c>
       <c r="AI26" s="3" t="s">
@@ -3115,7 +3116,7 @@
         <v>47</v>
       </c>
       <c r="AK26" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL26" s="3" t="s">
         <v>49</v>
@@ -3124,40 +3125,40 @@
       <c r="AN26" s="3"/>
     </row>
     <row r="27">
-      <c r="A27" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="23">
+      <c r="A27" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="22">
         <v>46.1</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="22">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E27" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="F27" s="24">
-        <v>143.2</v>
-      </c>
-      <c r="G27" s="24">
-        <v>-66.4</v>
-      </c>
-      <c r="H27" s="23">
-        <v>4447.8</v>
-      </c>
-      <c r="I27" s="24">
-        <v>3.8</v>
+      <c r="E27" s="23">
+        <v>8.0</v>
+      </c>
+      <c r="F27" s="23">
+        <v>161.8</v>
+      </c>
+      <c r="G27" s="23">
+        <v>-54.8</v>
+      </c>
+      <c r="H27" s="22">
+        <v>599.6</v>
+      </c>
+      <c r="I27" s="23">
+        <v>2.3</v>
       </c>
       <c r="J27" s="14"/>
-      <c r="K27" s="26">
-        <v>-65.2</v>
-      </c>
-      <c r="L27" s="26">
-        <v>-5.2</v>
+      <c r="K27" s="25">
+        <v>-72.6</v>
+      </c>
+      <c r="L27" s="25">
+        <v>-56.8</v>
       </c>
       <c r="M27" s="14"/>
       <c r="N27" s="14"/>
@@ -3186,10 +3187,10 @@
         <v>44</v>
       </c>
       <c r="Y27" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z27" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA27" s="17">
         <v>0.0</v>
@@ -3202,15 +3203,13 @@
         <v>0.0</v>
       </c>
       <c r="AE27" s="14"/>
-      <c r="AF27" s="18">
-        <v>4.0</v>
-      </c>
-      <c r="AG27" s="25">
+      <c r="AF27" s="17">
         <v>0.0</v>
       </c>
-      <c r="AH27" s="25">
-        <v>12.0</v>
-      </c>
+      <c r="AG27" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="AH27" s="14"/>
       <c r="AI27" s="3" t="s">
         <v>46</v>
       </c>
@@ -3218,7 +3217,7 @@
         <v>47</v>
       </c>
       <c r="AK27" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL27" s="3" t="s">
         <v>49</v>
@@ -3227,40 +3226,39 @@
       <c r="AN27" s="3"/>
     </row>
     <row r="28">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="20" t="s">
-        <v>67</v>
-      </c>
       <c r="C28" s="23">
-        <v>46.1</v>
+        <v>45.8</v>
       </c>
       <c r="D28" s="23">
-        <f t="shared" si="3"/>
-        <v>244.9</v>
-      </c>
-      <c r="E28" s="24">
-        <v>8.0</v>
-      </c>
-      <c r="F28" s="24">
-        <v>161.8</v>
-      </c>
-      <c r="G28" s="24">
-        <v>-54.8</v>
+        <v>246.1</v>
+      </c>
+      <c r="E28" s="23">
+        <v>7.0</v>
+      </c>
+      <c r="F28" s="23">
+        <v>270.1</v>
+      </c>
+      <c r="G28" s="23">
+        <v>-71.9</v>
       </c>
       <c r="H28" s="23">
-        <v>599.6</v>
-      </c>
-      <c r="I28" s="24">
-        <v>2.3</v>
+        <v>113.4</v>
+      </c>
+      <c r="I28" s="23">
+        <v>5.7</v>
       </c>
       <c r="J28" s="14"/>
-      <c r="K28" s="26">
-        <v>-72.6</v>
-      </c>
-      <c r="L28" s="26">
-        <v>-56.8</v>
+      <c r="K28" s="23">
+        <v>-36.8</v>
+      </c>
+      <c r="L28" s="23">
+        <v>108.3</v>
       </c>
       <c r="M28" s="14"/>
       <c r="N28" s="14"/>
@@ -3289,16 +3287,16 @@
         <v>44</v>
       </c>
       <c r="Y28" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z28" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA28" s="17">
         <v>0.0</v>
       </c>
-      <c r="AB28" s="17">
-        <v>1.0</v>
+      <c r="AB28" s="18">
+        <v>2.0</v>
       </c>
       <c r="AC28" s="14"/>
       <c r="AD28" s="17">
@@ -3308,10 +3306,12 @@
       <c r="AF28" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG28" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="AH28" s="14"/>
+      <c r="AG28" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="AH28" s="28">
+        <v>7.0</v>
+      </c>
       <c r="AI28" s="3" t="s">
         <v>46</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>47</v>
       </c>
       <c r="AK28" s="3" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="AL28" s="3" t="s">
         <v>49</v>
@@ -3328,39 +3328,39 @@
       <c r="AN28" s="3"/>
     </row>
     <row r="29">
-      <c r="A29" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="24">
-        <v>45.8</v>
-      </c>
-      <c r="D29" s="24">
+      <c r="A29" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="23">
+        <v>45.9</v>
+      </c>
+      <c r="D29" s="23">
         <v>246.1</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="23">
         <v>7.0</v>
       </c>
-      <c r="F29" s="24">
-        <v>270.1</v>
-      </c>
-      <c r="G29" s="24">
-        <v>-71.9</v>
-      </c>
-      <c r="H29" s="24">
-        <v>113.4</v>
-      </c>
-      <c r="I29" s="24">
-        <v>5.7</v>
+      <c r="F29" s="23">
+        <v>233.7</v>
+      </c>
+      <c r="G29" s="23">
+        <v>-60.3</v>
+      </c>
+      <c r="H29" s="23">
+        <v>99.7</v>
+      </c>
+      <c r="I29" s="23">
+        <v>6.1</v>
       </c>
       <c r="J29" s="14"/>
-      <c r="K29" s="24">
-        <v>-36.8</v>
-      </c>
-      <c r="L29" s="24">
-        <v>108.3</v>
+      <c r="K29" s="23">
+        <v>-51.5</v>
+      </c>
+      <c r="L29" s="23">
+        <v>142.8</v>
       </c>
       <c r="M29" s="14"/>
       <c r="N29" s="14"/>
@@ -3389,10 +3389,10 @@
         <v>44</v>
       </c>
       <c r="Y29" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z29" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA29" s="17">
         <v>0.0</v>
@@ -3408,10 +3408,12 @@
       <c r="AF29" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG29" s="25">
-        <v>2.0</v>
-      </c>
-      <c r="AH29" s="14"/>
+      <c r="AG29" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="AH29" s="28">
+        <v>7.0</v>
+      </c>
       <c r="AI29" s="3" t="s">
         <v>46</v>
       </c>
@@ -3419,7 +3421,7 @@
         <v>47</v>
       </c>
       <c r="AK29" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AL29" s="3" t="s">
         <v>49</v>
@@ -3427,40 +3429,40 @@
       <c r="AM29" s="3"/>
       <c r="AN29" s="3"/>
     </row>
-    <row r="30">
-      <c r="A30" s="22" t="s">
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="24">
+      <c r="B30" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="23">
         <v>45.9</v>
       </c>
-      <c r="D30" s="24">
-        <v>246.1</v>
-      </c>
-      <c r="E30" s="24">
-        <v>7.0</v>
-      </c>
-      <c r="F30" s="24">
-        <v>233.7</v>
-      </c>
-      <c r="G30" s="24">
-        <v>-60.3</v>
-      </c>
-      <c r="H30" s="24">
-        <v>99.7</v>
-      </c>
-      <c r="I30" s="24">
-        <v>6.1</v>
+      <c r="D30" s="23">
+        <v>246.2</v>
+      </c>
+      <c r="E30" s="23">
+        <v>6.0</v>
+      </c>
+      <c r="F30" s="23">
+        <v>350.9</v>
+      </c>
+      <c r="G30" s="23">
+        <v>67.8</v>
+      </c>
+      <c r="H30" s="23">
+        <v>138.0</v>
+      </c>
+      <c r="I30" s="23">
+        <v>5.7</v>
       </c>
       <c r="J30" s="14"/>
-      <c r="K30" s="24">
-        <v>-51.5</v>
-      </c>
-      <c r="L30" s="24">
-        <v>142.8</v>
+      <c r="K30" s="23">
+        <v>82.2</v>
+      </c>
+      <c r="L30" s="23">
+        <v>-161.5</v>
       </c>
       <c r="M30" s="14"/>
       <c r="N30" s="14"/>
@@ -3489,10 +3491,10 @@
         <v>44</v>
       </c>
       <c r="Y30" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z30" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA30" s="17">
         <v>0.0</v>
@@ -3508,10 +3510,12 @@
       <c r="AF30" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG30" s="25">
-        <v>2.0</v>
-      </c>
-      <c r="AH30" s="14"/>
+      <c r="AG30" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="AH30" s="28">
+        <v>7.0</v>
+      </c>
       <c r="AI30" s="3" t="s">
         <v>46</v>
       </c>
@@ -3519,7 +3523,7 @@
         <v>47</v>
       </c>
       <c r="AK30" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AL30" s="3" t="s">
         <v>49</v>
@@ -3528,39 +3532,39 @@
       <c r="AN30" s="3"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="24">
+      <c r="B31" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="23">
         <v>45.9</v>
       </c>
-      <c r="D31" s="24">
-        <v>246.2</v>
-      </c>
-      <c r="E31" s="24">
-        <v>6.0</v>
-      </c>
-      <c r="F31" s="24">
-        <v>350.9</v>
-      </c>
-      <c r="G31" s="24">
-        <v>67.8</v>
-      </c>
-      <c r="H31" s="24">
-        <v>138.0</v>
-      </c>
-      <c r="I31" s="24">
-        <v>5.7</v>
+      <c r="D31" s="23">
+        <v>246.3</v>
+      </c>
+      <c r="E31" s="23">
+        <v>5.0</v>
+      </c>
+      <c r="F31" s="23">
+        <v>100.5</v>
+      </c>
+      <c r="G31" s="23">
+        <v>75.0</v>
+      </c>
+      <c r="H31" s="23">
+        <v>142.8</v>
+      </c>
+      <c r="I31" s="23">
+        <v>6.4</v>
       </c>
       <c r="J31" s="14"/>
-      <c r="K31" s="24">
-        <v>82.2</v>
-      </c>
-      <c r="L31" s="24">
-        <v>-161.5</v>
+      <c r="K31" s="23">
+        <v>35.3</v>
+      </c>
+      <c r="L31" s="23">
+        <v>-79.8</v>
       </c>
       <c r="M31" s="14"/>
       <c r="N31" s="14"/>
@@ -3589,10 +3593,10 @@
         <v>44</v>
       </c>
       <c r="Y31" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z31" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA31" s="17">
         <v>0.0</v>
@@ -3608,10 +3612,12 @@
       <c r="AF31" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG31" s="25">
-        <v>2.0</v>
-      </c>
-      <c r="AH31" s="14"/>
+      <c r="AG31" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="AH31" s="28">
+        <v>7.0</v>
+      </c>
       <c r="AI31" s="3" t="s">
         <v>46</v>
       </c>
@@ -3619,7 +3625,7 @@
         <v>47</v>
       </c>
       <c r="AK31" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AL31" s="3" t="s">
         <v>49</v>
@@ -3628,39 +3634,39 @@
       <c r="AN31" s="3"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" s="24">
+      <c r="B32" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="23">
         <v>45.9</v>
       </c>
-      <c r="D32" s="24">
-        <v>246.3</v>
-      </c>
-      <c r="E32" s="24">
-        <v>5.0</v>
-      </c>
-      <c r="F32" s="24">
-        <v>100.5</v>
-      </c>
-      <c r="G32" s="24">
-        <v>75.0</v>
-      </c>
-      <c r="H32" s="24">
-        <v>142.8</v>
-      </c>
-      <c r="I32" s="24">
-        <v>6.4</v>
+      <c r="D32" s="23">
+        <v>246.2</v>
+      </c>
+      <c r="E32" s="23">
+        <v>6.0</v>
+      </c>
+      <c r="F32" s="23">
+        <v>90.6</v>
+      </c>
+      <c r="G32" s="23">
+        <v>79.1</v>
+      </c>
+      <c r="H32" s="23">
+        <v>247.3</v>
+      </c>
+      <c r="I32" s="23">
+        <v>4.3</v>
       </c>
       <c r="J32" s="14"/>
-      <c r="K32" s="24">
-        <v>35.3</v>
-      </c>
-      <c r="L32" s="24">
-        <v>-79.8</v>
+      <c r="K32" s="23">
+        <v>41.8</v>
+      </c>
+      <c r="L32" s="23">
+        <v>-84.8</v>
       </c>
       <c r="M32" s="14"/>
       <c r="N32" s="14"/>
@@ -3689,10 +3695,10 @@
         <v>44</v>
       </c>
       <c r="Y32" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z32" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA32" s="17">
         <v>0.0</v>
@@ -3708,10 +3714,12 @@
       <c r="AF32" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG32" s="25">
-        <v>2.0</v>
-      </c>
-      <c r="AH32" s="14"/>
+      <c r="AG32" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="AH32" s="28">
+        <v>7.0</v>
+      </c>
       <c r="AI32" s="3" t="s">
         <v>46</v>
       </c>
@@ -3719,7 +3727,7 @@
         <v>47</v>
       </c>
       <c r="AK32" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AL32" s="3" t="s">
         <v>49</v>
@@ -3728,39 +3736,39 @@
       <c r="AN32" s="3"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="24">
+      <c r="B33" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="23">
         <v>45.9</v>
       </c>
-      <c r="D33" s="24">
+      <c r="D33" s="23">
         <v>246.2</v>
       </c>
-      <c r="E33" s="24">
-        <v>6.0</v>
-      </c>
-      <c r="F33" s="24">
-        <v>90.6</v>
-      </c>
-      <c r="G33" s="24">
-        <v>79.1</v>
-      </c>
-      <c r="H33" s="24">
-        <v>247.3</v>
-      </c>
-      <c r="I33" s="24">
-        <v>4.3</v>
+      <c r="E33" s="23">
+        <v>5.0</v>
+      </c>
+      <c r="F33" s="23">
+        <v>197.2</v>
+      </c>
+      <c r="G33" s="23">
+        <v>-54.5</v>
+      </c>
+      <c r="H33" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="I33" s="23">
+        <v>11.0</v>
       </c>
       <c r="J33" s="14"/>
-      <c r="K33" s="24">
-        <v>41.8</v>
-      </c>
-      <c r="L33" s="24">
-        <v>-84.8</v>
+      <c r="K33" s="23">
+        <v>-73.3</v>
+      </c>
+      <c r="L33" s="23">
+        <v>-170.6</v>
       </c>
       <c r="M33" s="14"/>
       <c r="N33" s="14"/>
@@ -3789,10 +3797,10 @@
         <v>44</v>
       </c>
       <c r="Y33" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z33" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA33" s="17">
         <v>0.0</v>
@@ -3808,10 +3816,12 @@
       <c r="AF33" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG33" s="25">
-        <v>2.0</v>
-      </c>
-      <c r="AH33" s="14"/>
+      <c r="AG33" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="AH33" s="28">
+        <v>7.0</v>
+      </c>
       <c r="AI33" s="3" t="s">
         <v>46</v>
       </c>
@@ -3819,7 +3829,7 @@
         <v>47</v>
       </c>
       <c r="AK33" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AL33" s="3" t="s">
         <v>49</v>
@@ -3828,39 +3838,39 @@
       <c r="AN33" s="3"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="24">
-        <v>45.9</v>
-      </c>
-      <c r="D34" s="24">
-        <v>246.2</v>
-      </c>
-      <c r="E34" s="24">
-        <v>5.0</v>
-      </c>
-      <c r="F34" s="24">
-        <v>197.2</v>
-      </c>
-      <c r="G34" s="24">
-        <v>-54.5</v>
-      </c>
-      <c r="H34" s="24">
-        <v>49.5</v>
-      </c>
-      <c r="I34" s="24">
-        <v>11.0</v>
+      <c r="B34" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="23">
+        <v>46.1</v>
+      </c>
+      <c r="D34" s="23">
+        <v>246.0</v>
+      </c>
+      <c r="E34" s="23">
+        <v>3.0</v>
+      </c>
+      <c r="F34" s="23">
+        <v>186.2</v>
+      </c>
+      <c r="G34" s="23">
+        <v>-64.1</v>
+      </c>
+      <c r="H34" s="23">
+        <v>78.2</v>
+      </c>
+      <c r="I34" s="23">
+        <v>14.0</v>
       </c>
       <c r="J34" s="14"/>
-      <c r="K34" s="24">
-        <v>-73.3</v>
-      </c>
-      <c r="L34" s="24">
-        <v>-170.6</v>
+      <c r="K34" s="23">
+        <v>-86.1</v>
+      </c>
+      <c r="L34" s="23">
+        <v>154.8</v>
       </c>
       <c r="M34" s="14"/>
       <c r="N34" s="14"/>
@@ -3889,10 +3899,10 @@
         <v>44</v>
       </c>
       <c r="Y34" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z34" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA34" s="17">
         <v>0.0</v>
@@ -3908,10 +3918,12 @@
       <c r="AF34" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG34" s="25">
-        <v>2.0</v>
-      </c>
-      <c r="AH34" s="14"/>
+      <c r="AG34" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="AH34" s="28">
+        <v>7.0</v>
+      </c>
       <c r="AI34" s="3" t="s">
         <v>46</v>
       </c>
@@ -3919,7 +3931,7 @@
         <v>47</v>
       </c>
       <c r="AK34" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AL34" s="3" t="s">
         <v>49</v>
@@ -3928,39 +3940,39 @@
       <c r="AN34" s="3"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B35" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="24">
+      <c r="B35" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="23">
         <v>46.1</v>
       </c>
-      <c r="D35" s="24">
+      <c r="D35" s="23">
         <v>246.0</v>
       </c>
-      <c r="E35" s="24">
-        <v>3.0</v>
-      </c>
-      <c r="F35" s="24">
-        <v>186.2</v>
-      </c>
-      <c r="G35" s="24">
-        <v>-64.1</v>
-      </c>
-      <c r="H35" s="24">
-        <v>78.2</v>
-      </c>
-      <c r="I35" s="24">
-        <v>14.0</v>
+      <c r="E35" s="23">
+        <v>6.0</v>
+      </c>
+      <c r="F35" s="23">
+        <v>247.8</v>
+      </c>
+      <c r="G35" s="12">
+        <v>-44.9</v>
+      </c>
+      <c r="H35" s="23">
+        <v>596.3</v>
+      </c>
+      <c r="I35" s="23">
+        <v>2.8</v>
       </c>
       <c r="J35" s="14"/>
-      <c r="K35" s="24">
-        <v>-86.1</v>
-      </c>
-      <c r="L35" s="24">
-        <v>154.8</v>
+      <c r="K35" s="23">
+        <v>-33.8</v>
+      </c>
+      <c r="L35" s="12">
+        <v>151.5</v>
       </c>
       <c r="M35" s="14"/>
       <c r="N35" s="14"/>
@@ -3989,10 +4001,10 @@
         <v>44</v>
       </c>
       <c r="Y35" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z35" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA35" s="17">
         <v>0.0</v>
@@ -4008,10 +4020,12 @@
       <c r="AF35" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG35" s="25">
-        <v>2.0</v>
-      </c>
-      <c r="AH35" s="14"/>
+      <c r="AG35" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="AH35" s="28">
+        <v>7.0</v>
+      </c>
       <c r="AI35" s="3" t="s">
         <v>46</v>
       </c>
@@ -4019,7 +4033,7 @@
         <v>47</v>
       </c>
       <c r="AK35" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AL35" s="3" t="s">
         <v>49</v>
@@ -4028,127 +4042,55 @@
       <c r="AN35" s="3"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="24">
-        <v>46.1</v>
-      </c>
-      <c r="D36" s="24">
-        <v>246.0</v>
-      </c>
-      <c r="E36" s="24">
-        <v>6.0</v>
-      </c>
-      <c r="F36" s="24">
-        <v>247.8</v>
-      </c>
-      <c r="G36" s="12">
-        <v>-44.9</v>
-      </c>
-      <c r="H36" s="24">
-        <v>596.3</v>
-      </c>
-      <c r="I36" s="24">
-        <v>2.8</v>
-      </c>
-      <c r="J36" s="14"/>
-      <c r="K36" s="24">
-        <v>-33.8</v>
-      </c>
-      <c r="L36" s="12">
-        <v>151.5</v>
-      </c>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="16">
-        <v>46.4</v>
-      </c>
-      <c r="S36" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="T36" s="17">
-        <v>55.5</v>
-      </c>
-      <c r="U36" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="V36" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="W36" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="X36" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y36" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z36" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA36" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="AB36" s="18">
-        <v>2.0</v>
-      </c>
-      <c r="AC36" s="14"/>
-      <c r="AD36" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="AE36" s="14"/>
-      <c r="AF36" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="AG36" s="25">
-        <v>2.0</v>
-      </c>
-      <c r="AH36" s="14"/>
-      <c r="AI36" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ36" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK36" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AL36" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="3"/>
+      <c r="AC36" s="3"/>
+      <c r="AD36" s="3"/>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="3"/>
+      <c r="AG36" s="3"/>
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="3"/>
+      <c r="AJ36" s="3"/>
+      <c r="AK36" s="3"/>
+      <c r="AL36" s="3"/>
       <c r="AM36" s="3"/>
-      <c r="AN36" s="3"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="17"/>
+      <c r="B37" s="21"/>
       <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
       <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3"/>
-      <c r="S37" s="3"/>
-      <c r="T37" s="3"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="30"/>
+      <c r="S37" s="30"/>
+      <c r="T37" s="30"/>
       <c r="U37" s="3"/>
       <c r="V37" s="3"/>
-      <c r="W37" s="3"/>
-      <c r="X37" s="3"/>
+      <c r="W37" s="17"/>
+      <c r="X37" s="31"/>
       <c r="Y37" s="3"/>
-      <c r="Z37" s="3"/>
+      <c r="Z37" s="32"/>
       <c r="AA37" s="3"/>
       <c r="AB37" s="3"/>
       <c r="AC37" s="3"/>
@@ -4162,21 +4104,35 @@
       <c r="AK37" s="3"/>
       <c r="AL37" s="3"/>
       <c r="AM37" s="3"/>
+      <c r="AN37" s="3"/>
+      <c r="AO37" s="3"/>
+      <c r="AP37" s="3"/>
+      <c r="AQ37" s="3"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="B38" s="20"/>
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
       <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
       <c r="P38" s="3"/>
-      <c r="Q38" s="29"/>
-      <c r="R38" s="30"/>
-      <c r="S38" s="30"/>
-      <c r="T38" s="30"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
-      <c r="W38" s="17"/>
-      <c r="X38" s="31"/>
+      <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
       <c r="Y38" s="3"/>
-      <c r="Z38" s="32"/>
+      <c r="Z38" s="3"/>
       <c r="AA38" s="3"/>
       <c r="AB38" s="3"/>
       <c r="AC38" s="3"/>
@@ -4455,6 +4411,7 @@
       <c r="E45" s="3"/>
       <c r="G45" s="3"/>
       <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
@@ -4495,7 +4452,9 @@
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
       <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
@@ -47822,51 +47781,6 @@
       <c r="AP1008" s="3"/>
       <c r="AQ1008" s="3"/>
     </row>
-    <row r="1009" ht="15.75" customHeight="1">
-      <c r="A1009" s="3"/>
-      <c r="B1009" s="3"/>
-      <c r="C1009" s="3"/>
-      <c r="D1009" s="3"/>
-      <c r="E1009" s="3"/>
-      <c r="F1009" s="3"/>
-      <c r="G1009" s="3"/>
-      <c r="H1009" s="3"/>
-      <c r="I1009" s="3"/>
-      <c r="J1009" s="3"/>
-      <c r="K1009" s="3"/>
-      <c r="L1009" s="3"/>
-      <c r="M1009" s="3"/>
-      <c r="N1009" s="3"/>
-      <c r="O1009" s="3"/>
-      <c r="P1009" s="3"/>
-      <c r="Q1009" s="3"/>
-      <c r="R1009" s="3"/>
-      <c r="S1009" s="3"/>
-      <c r="T1009" s="3"/>
-      <c r="U1009" s="3"/>
-      <c r="V1009" s="3"/>
-      <c r="W1009" s="3"/>
-      <c r="X1009" s="3"/>
-      <c r="Y1009" s="3"/>
-      <c r="Z1009" s="3"/>
-      <c r="AA1009" s="3"/>
-      <c r="AB1009" s="3"/>
-      <c r="AC1009" s="3"/>
-      <c r="AD1009" s="3"/>
-      <c r="AE1009" s="3"/>
-      <c r="AF1009" s="3"/>
-      <c r="AG1009" s="3"/>
-      <c r="AH1009" s="3"/>
-      <c r="AI1009" s="3"/>
-      <c r="AJ1009" s="3"/>
-      <c r="AK1009" s="3"/>
-      <c r="AL1009" s="3"/>
-      <c r="AM1009" s="3"/>
-      <c r="AN1009" s="3"/>
-      <c r="AO1009" s="3"/>
-      <c r="AP1009" s="3"/>
-      <c r="AQ1009" s="3"/>
-    </row>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>